<commit_message>
changed icon and added QGIS support
</commit_message>
<xml_diff>
--- a/IconSource.xlsx
+++ b/IconSource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\FhrRasterSchweiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F188AFF2-D273-4742-A7C5-519901106FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB664E0-C3D6-4B7A-AD3A-B614AA5DB6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{A00CF303-3B93-4FA5-850C-D92727C4E32A}"/>
+    <workbookView xWindow="330" yWindow="1950" windowWidth="25560" windowHeight="20520" xr2:uid="{A00CF303-3B93-4FA5-850C-D92727C4E32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +92,25 @@
       <sz val="22"/>
       <color theme="1"/>
       <name val="_SwissArmy"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="0"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -120,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -144,12 +163,113 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -159,6 +279,60 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -168,6 +342,28 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -177,88 +373,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -267,50 +386,69 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,6 +464,133 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>33130</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57977</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>624093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D287612C-110C-36DE-1671-1F119EAB84CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10055087" y="231912"/>
+          <a:ext cx="4451488" cy="3067464"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>581025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79990DA1-CC3F-42C9-0188-F09BD15821BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10325100" y="3467100"/>
+          <a:ext cx="2295525" cy="2181225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -648,77 +913,74 @@
   <dimension ref="B1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M12"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="12.28515625" customWidth="1"/>
     <col min="13" max="13" width="5.140625" customWidth="1"/>
-    <col min="14" max="15" width="12.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="14" max="15" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="18" t="s">
+    <row r="2" spans="2:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
     </row>
-    <row r="3" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="3" t="s">
+    <row r="3" spans="2:13" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="B3" s="27"/>
+      <c r="C3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="9"/>
+      <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+    <row r="4" spans="2:13" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="B4" s="25">
+        <v>2</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -726,17 +988,17 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="11">
+      <c r="M4" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+    <row r="5" spans="2:13" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="1.05">
+      <c r="B5" s="26">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -744,16 +1006,16 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="13">
+      <c r="M5" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+    <row r="6" spans="2:13" ht="63" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="22">
         <v>6</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -762,12 +1024,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="11">
+      <c r="M6" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
@@ -780,12 +1042,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="13">
+      <c r="M7" s="8">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+      <c r="B8" s="5">
         <v>4</v>
       </c>
       <c r="C8" s="1"/>
@@ -798,12 +1060,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="11">
+      <c r="M8" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
+      <c r="B9" s="7">
         <v>3</v>
       </c>
       <c r="C9" s="1"/>
@@ -816,12 +1078,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="13">
+      <c r="M9" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
+      <c r="B10" s="5">
         <v>2</v>
       </c>
       <c r="C10" s="1"/>
@@ -834,12 +1096,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="11">
+      <c r="M10" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="B11" s="7">
         <v>1</v>
       </c>
       <c r="C11" s="1"/>
@@ -852,54 +1114,54 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="13">
+      <c r="M11" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="L12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="17"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B2:E2"/>
+  <mergeCells count="2">
     <mergeCell ref="J2:M2"/>
+    <mergeCell ref="D2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>